<commit_message>
Now setting worksheet names.
</commit_message>
<xml_diff>
--- a/data/psut_io_zaf_2013.xlsx
+++ b/data/psut_io_zaf_2013.xlsx
@@ -8,73 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C2243E-14EC-7243-8B32-894F67711B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91779313-04D9-9449-A525-BBF3FFA0BD75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="49560" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23560" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
-    <sheet name="2" sheetId="2" r:id="rId2"/>
+    <sheet name="ZAF-2013-E" sheetId="1" r:id="rId1"/>
+    <sheet name="ZAF-2013-X" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="R_1">'1'!$B$116:$AC$119</definedName>
-    <definedName name="R_2">'2'!$B$116:$AC$119</definedName>
-    <definedName name="r_eiou_1">'1'!$AX$2:$BK$29</definedName>
-    <definedName name="r_eiou_2">'2'!$AX$2:$BK$29</definedName>
-    <definedName name="S_units_1">'1'!$B$2:$B$33</definedName>
-    <definedName name="S_units_2">'2'!$B$2:$B$33</definedName>
-    <definedName name="U_1">'1'!$AG$66:$AT$93</definedName>
-    <definedName name="U_2">'2'!$AG$66:$AT$93</definedName>
-    <definedName name="U_eiou_1">'1'!$AG$2:$AT$29</definedName>
-    <definedName name="U_eiou_2">'2'!$AG$2:$AT$29</definedName>
-    <definedName name="U_feed_1">'1'!$AG$34:$AT$61</definedName>
-    <definedName name="U_feed_2">'2'!$AG$34:$AT$61</definedName>
-    <definedName name="V_1">'1'!$B$98:$AC$111</definedName>
-    <definedName name="V_2">'2'!$B$98:$AC$111</definedName>
-    <definedName name="Y_1">'1'!$AX$66:$BZ$93</definedName>
-    <definedName name="Y_2">'2'!$AX$66:$BZ$93</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="88">
   <si>
     <t/>
   </si>
@@ -339,33 +287,12 @@
   <si>
     <t>S_units</t>
   </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>(iR)^T</t>
-  </si>
-  <si>
-    <t>(iV)^T</t>
-  </si>
-  <si>
-    <t>–</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>Ui</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -386,16 +313,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -417,18 +336,6 @@
         <fgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -442,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -466,20 +373,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,15 +669,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CA155"/>
+  <dimension ref="A1:BZ120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="M149" sqref="M149"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
     <col min="2" max="29" width="7.6640625" customWidth="1"/>
     <col min="33" max="46" width="7.6640625" customWidth="1"/>
     <col min="50" max="78" width="7.6640625" customWidth="1"/>
@@ -1704,7 +1594,7 @@
         <v>0</v>
       </c>
       <c r="AN10" s="6">
-        <v>56051.467633337998</v>
+        <v>56051.467633338303</v>
       </c>
       <c r="AO10" s="6">
         <v>0</v>
@@ -1719,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="AS10" s="6">
-        <v>29853.109243252002</v>
+        <v>29853.1092432519</v>
       </c>
       <c r="AT10" s="6">
         <v>0</v>
@@ -2767,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="AI21" s="6">
-        <v>548828.21939997002</v>
+        <v>548828.21939996595</v>
       </c>
       <c r="AJ21" s="6">
         <v>0</v>
@@ -3287,7 +3177,7 @@
         <v>0</v>
       </c>
       <c r="AS26" s="6">
-        <v>39169.811628099</v>
+        <v>39169.811628099204</v>
       </c>
       <c r="AT26" s="6">
         <v>0</v>
@@ -3761,7 +3651,7 @@
         <v>0</v>
       </c>
       <c r="AJ34" s="6">
-        <v>84605.340351887993</v>
+        <v>84605.340351888095</v>
       </c>
       <c r="AK34" s="6">
         <v>0</v>
@@ -4043,7 +3933,7 @@
         <v>0</v>
       </c>
       <c r="AJ40" s="6">
-        <v>124511.39817072</v>
+        <v>124511.398170719</v>
       </c>
       <c r="AK40" s="6">
         <v>136378</v>
@@ -4114,7 +4004,7 @@
         <v>0</v>
       </c>
       <c r="AR41" s="6">
-        <v>2589.5469118602</v>
+        <v>2589.54691186016</v>
       </c>
       <c r="AS41" s="6">
         <v>819630.83316300996</v>
@@ -4290,7 +4180,7 @@
         <v>0</v>
       </c>
       <c r="AN45" s="6">
-        <v>1971.6652365325001</v>
+        <v>1971.6652365324701</v>
       </c>
       <c r="AO45" s="6">
         <v>0</v>
@@ -4337,10 +4227,10 @@
         <v>0</v>
       </c>
       <c r="AN46" s="6">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AO46" s="6">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AP46" s="6">
         <v>0</v>
@@ -4522,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="AM50" s="6">
-        <v>100281.38610904</v>
+        <v>100281.38610904101</v>
       </c>
       <c r="AN50" s="6">
         <v>0</v>
@@ -4531,7 +4421,7 @@
         <v>0</v>
       </c>
       <c r="AP50" s="6">
-        <v>43278.246086077997</v>
+        <v>43278.246086078099</v>
       </c>
       <c r="AQ50" s="6">
         <v>0</v>
@@ -4584,10 +4474,10 @@
         <v>0</v>
       </c>
       <c r="AR51" s="6">
-        <v>6084.0486357421996</v>
+        <v>6084.0486357421596</v>
       </c>
       <c r="AS51" s="6">
-        <v>6084.0486357421996</v>
+        <v>6084.0486357421596</v>
       </c>
       <c r="AT51" s="6">
         <v>0</v>
@@ -4622,13 +4512,13 @@
         <v>0</v>
       </c>
       <c r="AO52" s="6">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AP52" s="6">
         <v>0</v>
       </c>
       <c r="AQ52" s="6">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AR52" s="6">
         <v>0</v>
@@ -4651,22 +4541,22 @@
         <v>0</v>
       </c>
       <c r="AI53" s="6">
-        <v>208540.57520215999</v>
+        <v>208540.57520216401</v>
       </c>
       <c r="AJ53" s="6">
-        <v>5808678.6251109</v>
+        <v>5808678.62511086</v>
       </c>
       <c r="AK53" s="6">
         <v>0</v>
       </c>
       <c r="AL53" s="6">
-        <v>81743.889999998995</v>
+        <v>81743.889999999403</v>
       </c>
       <c r="AM53" s="6">
         <v>0</v>
       </c>
       <c r="AN53" s="6">
-        <v>2515807.1581589999</v>
+        <v>2515807.1581589798</v>
       </c>
       <c r="AO53" s="6">
         <v>0</v>
@@ -4731,7 +4621,7 @@
         <v>0</v>
       </c>
       <c r="AT54" s="6">
-        <v>204990.24277469999</v>
+        <v>204990.242774696</v>
       </c>
     </row>
     <row r="55" spans="32:46" x14ac:dyDescent="0.2">
@@ -4854,10 +4744,10 @@
         <v>0</v>
       </c>
       <c r="AN57" s="6">
-        <v>3653.5068995009001</v>
+        <v>3653.5068995009201</v>
       </c>
       <c r="AO57" s="6">
-        <v>283520.52911790001</v>
+        <v>283520.52911790402</v>
       </c>
       <c r="AP57" s="6">
         <v>0</v>
@@ -4951,7 +4841,7 @@
         <v>68.315984670820995</v>
       </c>
       <c r="AO59" s="6">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AP59" s="6">
         <v>0</v>
@@ -5042,10 +4932,10 @@
         <v>0</v>
       </c>
       <c r="AN61" s="6">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AO61" s="6">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AP61" s="6">
         <v>0</v>
@@ -5082,7 +4972,7 @@
       <c r="AS62" s="8"/>
       <c r="AT62" s="8"/>
     </row>
-    <row r="65" spans="32:79" ht="203" x14ac:dyDescent="0.2">
+    <row r="65" spans="32:78" ht="203" x14ac:dyDescent="0.2">
       <c r="AF65" s="3" t="s">
         <v>0</v>
       </c>
@@ -5219,7 +5109,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="32:79" x14ac:dyDescent="0.2">
+    <row r="66" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF66" s="4" t="s">
         <v>1</v>
       </c>
@@ -5233,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="AJ66" s="5">
-        <v>84605.340351887993</v>
+        <v>84605.340351888095</v>
       </c>
       <c r="AK66" s="5">
         <v>0</v>
@@ -5264,10 +5154,6 @@
       </c>
       <c r="AT66" s="5">
         <v>0</v>
-      </c>
-      <c r="AU66" s="11">
-        <f>SUM(AG66:AT66)</f>
-        <v>84605.340351887993</v>
       </c>
       <c r="AW66" s="4" t="s">
         <v>1</v>
@@ -5345,7 +5231,7 @@
         <v>0</v>
       </c>
       <c r="BV66" s="1">
-        <v>6882.63</v>
+        <v>6882.6300000000101</v>
       </c>
       <c r="BW66" s="1">
         <v>0</v>
@@ -5359,12 +5245,8 @@
       <c r="BZ66" s="1">
         <v>0</v>
       </c>
-      <c r="CA66" s="11">
-        <f>SUM(AX66:BZ66)</f>
-        <v>85444.74</v>
-      </c>
-    </row>
-    <row r="67" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF67" s="4" t="s">
         <v>2</v>
       </c>
@@ -5410,10 +5292,6 @@
       <c r="AT67" s="5">
         <v>0</v>
       </c>
-      <c r="AU67" s="11">
-        <f t="shared" ref="AU67:AU93" si="0">SUM(AG67:AT67)</f>
-        <v>0</v>
-      </c>
       <c r="AW67" s="4" t="s">
         <v>2</v>
       </c>
@@ -5490,7 +5368,7 @@
         <v>0</v>
       </c>
       <c r="BV67" s="1">
-        <v>1.0000000000105E-2</v>
+        <v>1.0000000000104601E-2</v>
       </c>
       <c r="BW67" s="1">
         <v>0</v>
@@ -5504,12 +5382,8 @@
       <c r="BZ67" s="1">
         <v>0</v>
       </c>
-      <c r="CA67" s="11">
-        <f t="shared" ref="CA67:CA93" si="1">SUM(AX67:BZ67)</f>
-        <v>1503.2200000000003</v>
-      </c>
-    </row>
-    <row r="68" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF68" s="4" t="s">
         <v>3</v>
       </c>
@@ -5555,10 +5429,6 @@
       <c r="AT68" s="5">
         <v>0</v>
       </c>
-      <c r="AU68" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW68" s="4" t="s">
         <v>3</v>
       </c>
@@ -5649,12 +5519,8 @@
       <c r="BZ68" s="1">
         <v>0</v>
       </c>
-      <c r="CA68" s="11">
-        <f t="shared" si="1"/>
-        <v>23509</v>
-      </c>
-    </row>
-    <row r="69" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF69" s="4" t="s">
         <v>4</v>
       </c>
@@ -5700,10 +5566,6 @@
       <c r="AT69" s="5">
         <v>0</v>
       </c>
-      <c r="AU69" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW69" s="4" t="s">
         <v>4</v>
       </c>
@@ -5794,12 +5656,8 @@
       <c r="BZ69" s="1">
         <v>0</v>
       </c>
-      <c r="CA69" s="11">
-        <f t="shared" si="1"/>
-        <v>17001.599999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF70" s="4" t="s">
         <v>5</v>
       </c>
@@ -5845,10 +5703,6 @@
       <c r="AT70" s="5">
         <v>0</v>
       </c>
-      <c r="AU70" s="11">
-        <f t="shared" si="0"/>
-        <v>58772.57</v>
-      </c>
       <c r="AW70" s="4" t="s">
         <v>5</v>
       </c>
@@ -5939,12 +5793,8 @@
       <c r="BZ70" s="1">
         <v>0</v>
       </c>
-      <c r="CA70" s="11">
-        <f t="shared" si="1"/>
-        <v>11182.16</v>
-      </c>
-    </row>
-    <row r="71" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF71" s="4" t="s">
         <v>6</v>
       </c>
@@ -5990,10 +5840,6 @@
       <c r="AT71" s="5">
         <v>0</v>
       </c>
-      <c r="AU71" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW71" s="4" t="s">
         <v>6</v>
       </c>
@@ -6084,12 +5930,8 @@
       <c r="BZ71" s="1">
         <v>0</v>
       </c>
-      <c r="CA71" s="11">
-        <f t="shared" si="1"/>
-        <v>25509.599999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF72" s="4" t="s">
         <v>7</v>
       </c>
@@ -6103,7 +5945,7 @@
         <v>0</v>
       </c>
       <c r="AJ72" s="5">
-        <v>124511.39817072</v>
+        <v>124511.398170719</v>
       </c>
       <c r="AK72" s="5">
         <v>136378</v>
@@ -6135,10 +5977,6 @@
       <c r="AT72" s="5">
         <v>0</v>
       </c>
-      <c r="AU72" s="11">
-        <f t="shared" si="0"/>
-        <v>260889.39817072</v>
-      </c>
       <c r="AW72" s="4" t="s">
         <v>7</v>
       </c>
@@ -6229,12 +6067,8 @@
       <c r="BZ72" s="1">
         <v>0</v>
       </c>
-      <c r="CA72" s="11">
-        <f t="shared" si="1"/>
-        <v>17729.14</v>
-      </c>
-    </row>
-    <row r="73" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF73" s="4" t="s">
         <v>8</v>
       </c>
@@ -6272,7 +6106,7 @@
         <v>0</v>
       </c>
       <c r="AR73" s="5">
-        <v>2589.5469118602</v>
+        <v>2589.54691186016</v>
       </c>
       <c r="AS73" s="5">
         <v>819630.83316300996</v>
@@ -6280,10 +6114,6 @@
       <c r="AT73" s="5">
         <v>0</v>
       </c>
-      <c r="AU73" s="11">
-        <f t="shared" si="0"/>
-        <v>822220.38007487019</v>
-      </c>
       <c r="AW73" s="4" t="s">
         <v>8</v>
       </c>
@@ -6374,12 +6204,8 @@
       <c r="BZ73" s="1">
         <v>0</v>
       </c>
-      <c r="CA73" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF74" s="4" t="s">
         <v>9</v>
       </c>
@@ -6405,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="AN74" s="5">
-        <v>56051.467633337998</v>
+        <v>56051.467633338303</v>
       </c>
       <c r="AO74" s="5">
         <v>0</v>
@@ -6420,14 +6246,10 @@
         <v>0</v>
       </c>
       <c r="AS74" s="5">
-        <v>29853.109243252002</v>
+        <v>29853.1092432519</v>
       </c>
       <c r="AT74" s="5">
         <v>0</v>
-      </c>
-      <c r="AU74" s="11">
-        <f t="shared" si="0"/>
-        <v>97500.331276368001</v>
       </c>
       <c r="AW74" s="4" t="s">
         <v>9</v>
@@ -6505,7 +6327,7 @@
         <v>104.4</v>
       </c>
       <c r="BV74" s="1">
-        <v>10774.8</v>
+        <v>10774.799999999899</v>
       </c>
       <c r="BW74" s="1">
         <v>450</v>
@@ -6519,12 +6341,8 @@
       <c r="BZ74" s="1">
         <v>1022.4</v>
       </c>
-      <c r="CA74" s="11">
-        <f t="shared" si="1"/>
-        <v>846770.4</v>
-      </c>
-    </row>
-    <row r="75" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF75" s="4" t="s">
         <v>10</v>
       </c>
@@ -6570,10 +6388,6 @@
       <c r="AT75" s="5">
         <v>0</v>
       </c>
-      <c r="AU75" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW75" s="4" t="s">
         <v>10</v>
       </c>
@@ -6664,12 +6478,8 @@
       <c r="BZ75" s="1">
         <v>0</v>
       </c>
-      <c r="CA75" s="11">
-        <f t="shared" si="1"/>
-        <v>147980.4</v>
-      </c>
-    </row>
-    <row r="76" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF76" s="4" t="s">
         <v>11</v>
       </c>
@@ -6715,10 +6525,6 @@
       <c r="AT76" s="5">
         <v>0</v>
       </c>
-      <c r="AU76" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW76" s="4" t="s">
         <v>11</v>
       </c>
@@ -6795,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="BV76" s="1">
-        <v>3.6379788070917E-12</v>
+        <v>3.6379788070917101E-12</v>
       </c>
       <c r="BW76" s="1">
         <v>0</v>
@@ -6809,12 +6615,8 @@
       <c r="BZ76" s="1">
         <v>0</v>
       </c>
-      <c r="CA76" s="11">
-        <f t="shared" si="1"/>
-        <v>21987.9</v>
-      </c>
-    </row>
-    <row r="77" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF77" s="4" t="s">
         <v>12</v>
       </c>
@@ -6840,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="AN77" s="5">
-        <v>1971.6652365325001</v>
+        <v>1971.6652365324701</v>
       </c>
       <c r="AO77" s="5">
         <v>0</v>
@@ -6859,10 +6661,6 @@
       </c>
       <c r="AT77" s="5">
         <v>0</v>
-      </c>
-      <c r="AU77" s="11">
-        <f t="shared" si="0"/>
-        <v>1971.6652365325001</v>
       </c>
       <c r="AW77" s="4" t="s">
         <v>12</v>
@@ -6940,7 +6738,7 @@
         <v>341946.72</v>
       </c>
       <c r="BV77" s="1">
-        <v>1.9999999960418999E-2</v>
+        <v>1.9999999960418801E-2</v>
       </c>
       <c r="BW77" s="1">
         <v>0</v>
@@ -6954,12 +6752,8 @@
       <c r="BZ77" s="1">
         <v>0</v>
       </c>
-      <c r="CA77" s="11">
-        <f t="shared" si="1"/>
-        <v>602183.29</v>
-      </c>
-    </row>
-    <row r="78" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF78" s="4" t="s">
         <v>13</v>
       </c>
@@ -6985,10 +6779,10 @@
         <v>0</v>
       </c>
       <c r="AN78" s="5">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AO78" s="5">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AP78" s="5">
         <v>0</v>
@@ -7004,10 +6798,6 @@
       </c>
       <c r="AT78" s="5">
         <v>0</v>
-      </c>
-      <c r="AU78" s="11">
-        <f t="shared" si="0"/>
-        <v>8039.7127223134003</v>
       </c>
       <c r="AW78" s="4" t="s">
         <v>13</v>
@@ -7099,12 +6889,8 @@
       <c r="BZ78" s="1">
         <v>0</v>
       </c>
-      <c r="CA78" s="11">
-        <f t="shared" si="1"/>
-        <v>2.8421709430404002E-13</v>
-      </c>
-    </row>
-    <row r="79" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF79" s="4" t="s">
         <v>14</v>
       </c>
@@ -7150,10 +6936,6 @@
       <c r="AT79" s="5">
         <v>0</v>
       </c>
-      <c r="AU79" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW79" s="4" t="s">
         <v>14</v>
       </c>
@@ -7230,7 +7012,7 @@
         <v>0</v>
       </c>
       <c r="BV79" s="1">
-        <v>7.2759576141834001E-12</v>
+        <v>7.2759576141834308E-12</v>
       </c>
       <c r="BW79" s="1">
         <v>0</v>
@@ -7244,12 +7026,8 @@
       <c r="BZ79" s="1">
         <v>0</v>
       </c>
-      <c r="CA79" s="11">
-        <f t="shared" si="1"/>
-        <v>79353.040000000008</v>
-      </c>
-    </row>
-    <row r="80" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF80" s="4" t="s">
         <v>15</v>
       </c>
@@ -7295,10 +7073,6 @@
       <c r="AT80" s="5">
         <v>0</v>
       </c>
-      <c r="AU80" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW80" s="4" t="s">
         <v>15</v>
       </c>
@@ -7389,12 +7163,8 @@
       <c r="BZ80" s="1">
         <v>0</v>
       </c>
-      <c r="CA80" s="11">
-        <f t="shared" si="1"/>
-        <v>14310.71</v>
-      </c>
-    </row>
-    <row r="81" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF81" s="4" t="s">
         <v>16</v>
       </c>
@@ -7440,10 +7210,6 @@
       <c r="AT81" s="5">
         <v>0</v>
       </c>
-      <c r="AU81" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW81" s="4" t="s">
         <v>16</v>
       </c>
@@ -7534,12 +7300,8 @@
       <c r="BZ81" s="1">
         <v>0</v>
       </c>
-      <c r="CA81" s="11">
-        <f t="shared" si="1"/>
-        <v>422743.92000000004</v>
-      </c>
-    </row>
-    <row r="82" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF82" s="4" t="s">
         <v>17</v>
       </c>
@@ -7562,7 +7324,7 @@
         <v>0</v>
       </c>
       <c r="AM82" s="5">
-        <v>100281.38610904</v>
+        <v>100281.38610904101</v>
       </c>
       <c r="AN82" s="5">
         <v>0</v>
@@ -7571,7 +7333,7 @@
         <v>0</v>
       </c>
       <c r="AP82" s="5">
-        <v>43278.246086077997</v>
+        <v>43278.246086078099</v>
       </c>
       <c r="AQ82" s="5">
         <v>0</v>
@@ -7584,10 +7346,6 @@
       </c>
       <c r="AT82" s="5">
         <v>0</v>
-      </c>
-      <c r="AU82" s="11">
-        <f t="shared" si="0"/>
-        <v>143559.632195118</v>
       </c>
       <c r="AW82" s="4" t="s">
         <v>17</v>
@@ -7665,7 +7423,7 @@
         <v>7.2</v>
       </c>
       <c r="BV82" s="1">
-        <v>1.4551915228367E-11</v>
+        <v>1.45519152283669E-11</v>
       </c>
       <c r="BW82" s="1">
         <v>9</v>
@@ -7679,12 +7437,8 @@
       <c r="BZ82" s="1">
         <v>0</v>
       </c>
-      <c r="CA82" s="11">
-        <f t="shared" si="1"/>
-        <v>71415</v>
-      </c>
-    </row>
-    <row r="83" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF83" s="4" t="s">
         <v>18</v>
       </c>
@@ -7722,17 +7476,13 @@
         <v>0</v>
       </c>
       <c r="AR83" s="5">
-        <v>6084.0486357421996</v>
+        <v>6084.0486357421596</v>
       </c>
       <c r="AS83" s="5">
-        <v>6084.0486357421996</v>
+        <v>6084.0486357421596</v>
       </c>
       <c r="AT83" s="5">
         <v>0</v>
-      </c>
-      <c r="AU83" s="11">
-        <f t="shared" si="0"/>
-        <v>12168.097271484399</v>
       </c>
       <c r="AW83" s="4" t="s">
         <v>18</v>
@@ -7824,12 +7574,8 @@
       <c r="BZ83" s="1">
         <v>0</v>
       </c>
-      <c r="CA83" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF84" s="4" t="s">
         <v>19</v>
       </c>
@@ -7858,13 +7604,13 @@
         <v>0</v>
       </c>
       <c r="AO84" s="5">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AP84" s="5">
         <v>0</v>
       </c>
       <c r="AQ84" s="5">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AR84" s="5">
         <v>0</v>
@@ -7874,10 +7620,6 @@
       </c>
       <c r="AT84" s="5">
         <v>0</v>
-      </c>
-      <c r="AU84" s="11">
-        <f t="shared" si="0"/>
-        <v>307389.25120847998</v>
       </c>
       <c r="AW84" s="4" t="s">
         <v>19</v>
@@ -7969,12 +7711,8 @@
       <c r="BZ84" s="1">
         <v>0</v>
       </c>
-      <c r="CA84" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF85" s="4" t="s">
         <v>20</v>
       </c>
@@ -7985,22 +7723,22 @@
         <v>0</v>
       </c>
       <c r="AI85" s="5">
-        <v>757368.79460212996</v>
+        <v>757368.79460212903</v>
       </c>
       <c r="AJ85" s="5">
-        <v>5808678.6251109</v>
+        <v>5808678.62511086</v>
       </c>
       <c r="AK85" s="5">
         <v>0</v>
       </c>
       <c r="AL85" s="5">
-        <v>81743.889999998995</v>
+        <v>81743.889999999403</v>
       </c>
       <c r="AM85" s="5">
         <v>0</v>
       </c>
       <c r="AN85" s="5">
-        <v>2515807.1581589999</v>
+        <v>2515807.1581589798</v>
       </c>
       <c r="AO85" s="5">
         <v>0</v>
@@ -8019,10 +7757,6 @@
       </c>
       <c r="AT85" s="5">
         <v>0</v>
-      </c>
-      <c r="AU85" s="11">
-        <f t="shared" si="0"/>
-        <v>9163598.4678720273</v>
       </c>
       <c r="AW85" s="4" t="s">
         <v>20</v>
@@ -8114,12 +7848,8 @@
       <c r="BZ85" s="1">
         <v>0</v>
       </c>
-      <c r="CA85" s="11">
-        <f t="shared" si="1"/>
-        <v>2601483.7399999998</v>
-      </c>
-    </row>
-    <row r="86" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF86" s="4" t="s">
         <v>21</v>
       </c>
@@ -8163,11 +7893,7 @@
         <v>0</v>
       </c>
       <c r="AT86" s="5">
-        <v>204990.24277469999</v>
-      </c>
-      <c r="AU86" s="11">
-        <f t="shared" si="0"/>
-        <v>204990.24277469999</v>
+        <v>204990.242774696</v>
       </c>
       <c r="AW86" s="4" t="s">
         <v>21</v>
@@ -8259,12 +7985,8 @@
       <c r="BZ86" s="1">
         <v>0</v>
       </c>
-      <c r="CA86" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF87" s="4" t="s">
         <v>22</v>
       </c>
@@ -8310,10 +8032,6 @@
       <c r="AT87" s="5">
         <v>0</v>
       </c>
-      <c r="AU87" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW87" s="4" t="s">
         <v>22</v>
       </c>
@@ -8404,12 +8122,8 @@
       <c r="BZ87" s="1">
         <v>0</v>
       </c>
-      <c r="CA87" s="11">
-        <f t="shared" si="1"/>
-        <v>21149.25</v>
-      </c>
-    </row>
-    <row r="88" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF88" s="4" t="s">
         <v>23</v>
       </c>
@@ -8455,10 +8169,6 @@
       <c r="AT88" s="5">
         <v>0</v>
       </c>
-      <c r="AU88" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="AW88" s="4" t="s">
         <v>23</v>
       </c>
@@ -8549,12 +8259,8 @@
       <c r="BZ88" s="1">
         <v>0</v>
       </c>
-      <c r="CA88" s="11">
-        <f t="shared" si="1"/>
-        <v>6880</v>
-      </c>
-    </row>
-    <row r="89" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF89" s="4" t="s">
         <v>24</v>
       </c>
@@ -8580,10 +8286,10 @@
         <v>0</v>
       </c>
       <c r="AN89" s="5">
-        <v>3653.5068995009001</v>
+        <v>3653.5068995009201</v>
       </c>
       <c r="AO89" s="5">
-        <v>283520.52911790001</v>
+        <v>283520.52911790402</v>
       </c>
       <c r="AP89" s="5">
         <v>0</v>
@@ -8599,10 +8305,6 @@
       </c>
       <c r="AT89" s="5">
         <v>0</v>
-      </c>
-      <c r="AU89" s="11">
-        <f t="shared" si="0"/>
-        <v>383681.03601740091</v>
       </c>
       <c r="AW89" s="4" t="s">
         <v>24</v>
@@ -8694,12 +8396,8 @@
       <c r="BZ89" s="1">
         <v>0</v>
       </c>
-      <c r="CA89" s="11">
-        <f t="shared" si="1"/>
-        <v>184769</v>
-      </c>
-    </row>
-    <row r="90" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF90" s="4" t="s">
         <v>25</v>
       </c>
@@ -8740,14 +8438,10 @@
         <v>0</v>
       </c>
       <c r="AS90" s="5">
-        <v>39169.811628099</v>
+        <v>39169.811628099204</v>
       </c>
       <c r="AT90" s="5">
         <v>0</v>
-      </c>
-      <c r="AU90" s="11">
-        <f t="shared" si="0"/>
-        <v>39169.811628099</v>
       </c>
       <c r="AW90" s="4" t="s">
         <v>25</v>
@@ -8839,12 +8533,8 @@
       <c r="BZ90" s="1">
         <v>0</v>
       </c>
-      <c r="CA90" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF91" s="4" t="s">
         <v>26</v>
       </c>
@@ -8873,7 +8563,7 @@
         <v>68.315984670820995</v>
       </c>
       <c r="AO91" s="5">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AP91" s="5">
         <v>0</v>
@@ -8889,10 +8579,6 @@
       </c>
       <c r="AT91" s="5">
         <v>0</v>
-      </c>
-      <c r="AU91" s="11">
-        <f t="shared" si="0"/>
-        <v>136.63196934164199</v>
       </c>
       <c r="AW91" s="4" t="s">
         <v>26</v>
@@ -8984,12 +8670,8 @@
       <c r="BZ91" s="1">
         <v>0</v>
       </c>
-      <c r="CA91" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF92" s="4" t="s">
         <v>27</v>
       </c>
@@ -9035,10 +8717,6 @@
       <c r="AT92" s="5">
         <v>0</v>
       </c>
-      <c r="AU92" s="11">
-        <f t="shared" si="0"/>
-        <v>3804</v>
-      </c>
       <c r="AW92" s="4" t="s">
         <v>27</v>
       </c>
@@ -9129,12 +8807,8 @@
       <c r="BZ92" s="1">
         <v>0</v>
       </c>
-      <c r="CA92" s="11">
-        <f t="shared" si="1"/>
-        <v>3804</v>
-      </c>
-    </row>
-    <row r="93" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF93" s="4" t="s">
         <v>28</v>
       </c>
@@ -9160,10 +8834,10 @@
         <v>0</v>
       </c>
       <c r="AN93" s="5">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AO93" s="5">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AP93" s="5">
         <v>0</v>
@@ -9179,10 +8853,6 @@
       </c>
       <c r="AT93" s="5">
         <v>0</v>
-      </c>
-      <c r="AU93" s="11">
-        <f t="shared" si="0"/>
-        <v>71.911562811389999</v>
       </c>
       <c r="AW93" s="4" t="s">
         <v>28</v>
@@ -9274,12 +8944,8 @@
       <c r="BZ93" s="1">
         <v>0</v>
       </c>
-      <c r="CA93" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="32:79" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="32:78" x14ac:dyDescent="0.2">
       <c r="AF94" s="4"/>
       <c r="AG94" s="7" t="s">
         <v>48</v>
@@ -9297,9 +8963,6 @@
       <c r="AR94" s="8"/>
       <c r="AS94" s="8"/>
       <c r="AT94" s="8"/>
-      <c r="AU94" s="12" t="s">
-        <v>93</v>
-      </c>
       <c r="AW94" s="4"/>
       <c r="AX94" s="7" t="s">
         <v>78</v>
@@ -9332,9 +8995,6 @@
       <c r="BX94" s="8"/>
       <c r="BY94" s="8"/>
       <c r="BZ94" s="8"/>
-      <c r="CA94" s="12" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="97" spans="1:29" ht="167" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
@@ -9668,7 +9328,7 @@
         <v>0</v>
       </c>
       <c r="V100" s="5">
-        <v>151544.47676958999</v>
+        <v>151544.47676959101</v>
       </c>
       <c r="W100" s="5">
         <v>0</v>
@@ -9754,7 +9414,7 @@
         <v>0</v>
       </c>
       <c r="U101" s="5">
-        <v>5806603.9036335004</v>
+        <v>5806603.9036334697</v>
       </c>
       <c r="V101" s="5">
         <v>0</v>
@@ -9905,7 +9565,7 @@
         <v>0</v>
       </c>
       <c r="L103" s="5">
-        <v>21987.9</v>
+        <v>21987.899999999801</v>
       </c>
       <c r="M103" s="5">
         <v>0</v>
@@ -10024,7 +9684,7 @@
         <v>0</v>
       </c>
       <c r="V104" s="5">
-        <v>53445.766005104</v>
+        <v>53445.766005104502</v>
       </c>
       <c r="W104" s="5">
         <v>0</v>
@@ -10077,7 +9737,7 @@
         <v>0</v>
       </c>
       <c r="J105" s="5">
-        <v>859652.39411768003</v>
+        <v>859652.39411767898</v>
       </c>
       <c r="K105" s="5">
         <v>0</v>
@@ -10178,7 +9838,7 @@
         <v>0</v>
       </c>
       <c r="N106" s="5">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="O106" s="5">
         <v>0</v>
@@ -10196,7 +9856,7 @@
         <v>0</v>
       </c>
       <c r="T106" s="5">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="U106" s="5">
         <v>0</v>
@@ -10211,19 +9871,19 @@
         <v>0</v>
       </c>
       <c r="Y106" s="5">
-        <v>283520.52911790001</v>
+        <v>283520.52911790402</v>
       </c>
       <c r="Z106" s="5">
         <v>0</v>
       </c>
       <c r="AA106" s="5">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AB106" s="5">
         <v>3804</v>
       </c>
       <c r="AC106" s="5">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.2">
@@ -10279,7 +9939,7 @@
         <v>0</v>
       </c>
       <c r="R107" s="5">
-        <v>43278.246086077997</v>
+        <v>43278.246086078099</v>
       </c>
       <c r="S107" s="5">
         <v>0</v>
@@ -10344,7 +10004,7 @@
         <v>0</v>
       </c>
       <c r="J108" s="5">
-        <v>50719.226449399997</v>
+        <v>50719.226449399699</v>
       </c>
       <c r="K108" s="5">
         <v>0</v>
@@ -10430,7 +10090,7 @@
         <v>0</v>
       </c>
       <c r="I109" s="5">
-        <v>2589.5469118602</v>
+        <v>2589.54691186016</v>
       </c>
       <c r="J109" s="5">
         <v>0</v>
@@ -10460,7 +10120,7 @@
         <v>0</v>
       </c>
       <c r="S109" s="5">
-        <v>6084.0486357421996</v>
+        <v>6084.0486357421596</v>
       </c>
       <c r="T109" s="5">
         <v>0</v>
@@ -10564,13 +10224,13 @@
         <v>18338</v>
       </c>
       <c r="X110" s="5">
-        <v>114.77006311993</v>
+        <v>114.770063119928</v>
       </c>
       <c r="Y110" s="5">
         <v>0</v>
       </c>
       <c r="Z110" s="5">
-        <v>39169.811628099</v>
+        <v>39169.811628099204</v>
       </c>
       <c r="AA110" s="5">
         <v>0</v>
@@ -10620,7 +10280,7 @@
         <v>0</v>
       </c>
       <c r="M111" s="5">
-        <v>116599.59202994</v>
+        <v>116599.592029939</v>
       </c>
       <c r="N111" s="5">
         <v>0</v>
@@ -10704,120 +10364,6 @@
       <c r="AB112" s="8"/>
       <c r="AC112" s="8"/>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B113" s="11">
-        <f>SUM(B98:B111)</f>
-        <v>85444.74</v>
-      </c>
-      <c r="C113" s="11">
-        <f t="shared" ref="C113:AC113" si="2">SUM(C98:C111)</f>
-        <v>0</v>
-      </c>
-      <c r="D113" s="11">
-        <f t="shared" si="2"/>
-        <v>23509</v>
-      </c>
-      <c r="E113" s="11">
-        <f t="shared" si="2"/>
-        <v>14476</v>
-      </c>
-      <c r="F113" s="11">
-        <f t="shared" si="2"/>
-        <v>69954.720000000001</v>
-      </c>
-      <c r="G113" s="11">
-        <f t="shared" si="2"/>
-        <v>25509.599999999999</v>
-      </c>
-      <c r="H113" s="11">
-        <f t="shared" si="2"/>
-        <v>125746.72</v>
-      </c>
-      <c r="I113" s="11">
-        <f t="shared" si="2"/>
-        <v>2589.5469118602</v>
-      </c>
-      <c r="J113" s="11">
-        <f t="shared" si="2"/>
-        <v>910371.62056707998</v>
-      </c>
-      <c r="K113" s="11">
-        <f t="shared" si="2"/>
-        <v>140326.23000000001</v>
-      </c>
-      <c r="L113" s="11">
-        <f t="shared" si="2"/>
-        <v>21987.9</v>
-      </c>
-      <c r="M113" s="11">
-        <f t="shared" si="2"/>
-        <v>419320.78706465999</v>
-      </c>
-      <c r="N113" s="11">
-        <f t="shared" si="2"/>
-        <v>4019.8563611567001</v>
-      </c>
-      <c r="O113" s="11">
-        <f t="shared" si="2"/>
-        <v>71713.460000000006</v>
-      </c>
-      <c r="P113" s="11">
-        <f t="shared" si="2"/>
-        <v>12159.42</v>
-      </c>
-      <c r="Q113" s="11">
-        <f t="shared" si="2"/>
-        <v>341568.97000000003</v>
-      </c>
-      <c r="R113" s="11">
-        <f t="shared" si="2"/>
-        <v>43278.246086077997</v>
-      </c>
-      <c r="S113" s="11">
-        <f t="shared" si="2"/>
-        <v>6084.0486357421996</v>
-      </c>
-      <c r="T113" s="11">
-        <f t="shared" si="2"/>
-        <v>153694.62560423999</v>
-      </c>
-      <c r="U113" s="11">
-        <f t="shared" si="2"/>
-        <v>5806603.9036335004</v>
-      </c>
-      <c r="V113" s="11">
-        <f t="shared" si="2"/>
-        <v>204990.24277469399</v>
-      </c>
-      <c r="W113" s="11">
-        <f t="shared" si="2"/>
-        <v>18338</v>
-      </c>
-      <c r="X113" s="11">
-        <f t="shared" si="2"/>
-        <v>114.77006311993</v>
-      </c>
-      <c r="Y113" s="11">
-        <f t="shared" si="2"/>
-        <v>283520.52911790001</v>
-      </c>
-      <c r="Z113" s="11">
-        <f t="shared" si="2"/>
-        <v>39169.811628099</v>
-      </c>
-      <c r="AA113" s="11">
-        <f t="shared" si="2"/>
-        <v>68.315984670820995</v>
-      </c>
-      <c r="AB113" s="11">
-        <f t="shared" si="2"/>
-        <v>3804</v>
-      </c>
-      <c r="AC113" s="11">
-        <f t="shared" si="2"/>
-        <v>35.955781405694999</v>
-      </c>
-    </row>
     <row r="115" spans="1:29" ht="167" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>0</v>
@@ -10933,10 +10479,10 @@
         <v>28360.42</v>
       </c>
       <c r="I116" s="1">
-        <v>732057.06487101002</v>
+        <v>732057.064871012</v>
       </c>
       <c r="J116" s="1">
-        <v>33899.110709289998</v>
+        <v>33899.110709289598</v>
       </c>
       <c r="K116" s="1">
         <v>4433.5600000000004</v>
@@ -10945,7 +10491,7 @@
         <v>0</v>
       </c>
       <c r="M116" s="1">
-        <v>184834.16817187</v>
+        <v>184834.16817187399</v>
       </c>
       <c r="N116" s="1">
         <v>0</v>
@@ -10957,10 +10503,10 @@
         <v>1870.68</v>
       </c>
       <c r="Q116" s="1">
-        <v>49154.22</v>
+        <v>49154.220000000103</v>
       </c>
       <c r="R116" s="1">
-        <v>128418.14002296</v>
+        <v>128418.14002296299</v>
       </c>
       <c r="S116" s="1">
         <v>0</v>
@@ -10978,10 +10524,10 @@
         <v>0</v>
       </c>
       <c r="X116" s="1">
-        <v>6765.2299368800996</v>
+        <v>6765.2299368800705</v>
       </c>
       <c r="Y116" s="1">
-        <v>1408.9777815964001</v>
+        <v>1408.9777815964201</v>
       </c>
       <c r="Z116" s="1">
         <v>0</v>
@@ -11001,7 +10547,7 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>84605.340351887993</v>
+        <v>84605.340351888095</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -11019,10 +10565,10 @@
         <v>0</v>
       </c>
       <c r="H117" s="1">
-        <v>124511.39817072</v>
+        <v>124511.398170719</v>
       </c>
       <c r="I117" s="1">
-        <v>2589.5469118602</v>
+        <v>2589.54691186016</v>
       </c>
       <c r="J117" s="1">
         <v>0</v>
@@ -11037,7 +10583,7 @@
         <v>0</v>
       </c>
       <c r="N117" s="1">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="O117" s="1">
         <v>0</v>
@@ -11049,16 +10595,16 @@
         <v>0</v>
       </c>
       <c r="R117" s="1">
-        <v>43278.246086077997</v>
+        <v>43278.246086078099</v>
       </c>
       <c r="S117" s="1">
-        <v>6084.0486357421996</v>
+        <v>6084.0486357421596</v>
       </c>
       <c r="T117" s="1">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="U117" s="1">
-        <v>5808678.6251109</v>
+        <v>5808678.62511086</v>
       </c>
       <c r="V117" s="1">
         <v>0</v>
@@ -11070,19 +10616,19 @@
         <v>0</v>
       </c>
       <c r="Y117" s="1">
-        <v>283520.52911790001</v>
+        <v>283520.52911790402</v>
       </c>
       <c r="Z117" s="1">
         <v>0</v>
       </c>
       <c r="AA117" s="1">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AB117" s="1">
         <v>3804</v>
       </c>
       <c r="AC117" s="1">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.2">
@@ -11102,7 +10648,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="1">
-        <v>9.9999999911233005E-3</v>
+        <v>9.99999999112333E-3</v>
       </c>
       <c r="G118" s="1">
         <v>0</v>
@@ -11111,13 +10657,13 @@
         <v>0</v>
       </c>
       <c r="I118" s="1">
-        <v>79334.300845170001</v>
+        <v>79334.300845170306</v>
       </c>
       <c r="J118" s="1">
         <v>0</v>
       </c>
       <c r="K118" s="1">
-        <v>3220.61</v>
+        <v>3220.6099999999901</v>
       </c>
       <c r="L118" s="1">
         <v>0</v>
@@ -11147,7 +10693,7 @@
         <v>0</v>
       </c>
       <c r="U118" s="1">
-        <v>149799.67912764</v>
+        <v>149799.67912763901</v>
       </c>
       <c r="V118" s="1">
         <v>0</v>
@@ -11200,7 +10746,7 @@
         <v>0</v>
       </c>
       <c r="I119" s="1">
-        <v>5649.9205349676004</v>
+        <v>5649.9205349676204</v>
       </c>
       <c r="J119" s="1">
         <v>0</v>
@@ -11295,796 +10841,6 @@
       <c r="AA120" s="8"/>
       <c r="AB120" s="8"/>
       <c r="AC120" s="8"/>
-    </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B121" s="11">
-        <f>SUM(B116:B119)</f>
-        <v>84605.340351887993</v>
-      </c>
-      <c r="C121" s="11">
-        <f t="shared" ref="C121:AC121" si="3">SUM(C116:C119)</f>
-        <v>1503.22</v>
-      </c>
-      <c r="D121" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="E121" s="11">
-        <f t="shared" si="3"/>
-        <v>2525.6</v>
-      </c>
-      <c r="F121" s="11">
-        <f t="shared" si="3"/>
-        <v>9.9999999911233005E-3</v>
-      </c>
-      <c r="G121" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H121" s="11">
-        <f t="shared" si="3"/>
-        <v>152871.81817072001</v>
-      </c>
-      <c r="I121" s="11">
-        <f t="shared" si="3"/>
-        <v>819630.83316300786</v>
-      </c>
-      <c r="J121" s="11">
-        <f t="shared" si="3"/>
-        <v>33899.110709289998</v>
-      </c>
-      <c r="K121" s="11">
-        <f t="shared" si="3"/>
-        <v>7654.17</v>
-      </c>
-      <c r="L121" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M121" s="11">
-        <f t="shared" si="3"/>
-        <v>184834.16817187</v>
-      </c>
-      <c r="N121" s="11">
-        <f t="shared" si="3"/>
-        <v>4019.8563611567001</v>
-      </c>
-      <c r="O121" s="11">
-        <f t="shared" si="3"/>
-        <v>7639.58</v>
-      </c>
-      <c r="P121" s="11">
-        <f t="shared" si="3"/>
-        <v>2151.29</v>
-      </c>
-      <c r="Q121" s="11">
-        <f t="shared" si="3"/>
-        <v>81174.95</v>
-      </c>
-      <c r="R121" s="11">
-        <f t="shared" si="3"/>
-        <v>171696.38610903799</v>
-      </c>
-      <c r="S121" s="11">
-        <f t="shared" si="3"/>
-        <v>6084.0486357421996</v>
-      </c>
-      <c r="T121" s="11">
-        <f t="shared" si="3"/>
-        <v>153694.62560423999</v>
-      </c>
-      <c r="U121" s="11">
-        <f t="shared" si="3"/>
-        <v>5958478.3042385401</v>
-      </c>
-      <c r="V121" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="W121" s="11">
-        <f t="shared" si="3"/>
-        <v>2811.25</v>
-      </c>
-      <c r="X121" s="11">
-        <f t="shared" si="3"/>
-        <v>6765.2299368800996</v>
-      </c>
-      <c r="Y121" s="11">
-        <f t="shared" si="3"/>
-        <v>284929.50689949642</v>
-      </c>
-      <c r="Z121" s="11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AA121" s="11">
-        <f t="shared" si="3"/>
-        <v>68.315984670820995</v>
-      </c>
-      <c r="AB121" s="11">
-        <f t="shared" si="3"/>
-        <v>3804</v>
-      </c>
-      <c r="AC121" s="11">
-        <f t="shared" si="3"/>
-        <v>35.955781405694999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B127" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C127" s="11" cm="1">
-        <f t="array" ref="C127:C154">TRANSPOSE(B121:AC121)</f>
-        <v>84605.340351887993</v>
-      </c>
-      <c r="E127" s="11" cm="1">
-        <f t="array" ref="E127:E154">TRANSPOSE(B113:AC113)</f>
-        <v>85444.74</v>
-      </c>
-      <c r="G127" s="11">
-        <f>AU66</f>
-        <v>84605.340351887993</v>
-      </c>
-      <c r="I127" s="11">
-        <f>CA66</f>
-        <v>85444.74</v>
-      </c>
-      <c r="K127" s="14">
-        <f>C127+E127-G127-I127</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B128" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C128" s="11">
-        <v>1503.22</v>
-      </c>
-      <c r="E128" s="11">
-        <v>0</v>
-      </c>
-      <c r="G128" s="11">
-        <f t="shared" ref="G128:G154" si="4">AU67</f>
-        <v>0</v>
-      </c>
-      <c r="I128" s="11">
-        <f t="shared" ref="I128:I154" si="5">CA67</f>
-        <v>1503.2200000000003</v>
-      </c>
-      <c r="K128" s="14">
-        <f t="shared" ref="K128:K154" si="6">C128+E128-G128-I128</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B129" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C129" s="11">
-        <v>0</v>
-      </c>
-      <c r="E129" s="11">
-        <v>23509</v>
-      </c>
-      <c r="G129" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I129" s="11">
-        <f t="shared" si="5"/>
-        <v>23509</v>
-      </c>
-      <c r="K129" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B130" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C130" s="11">
-        <v>2525.6</v>
-      </c>
-      <c r="E130" s="11">
-        <v>14476</v>
-      </c>
-      <c r="G130" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I130" s="11">
-        <f t="shared" si="5"/>
-        <v>17001.599999999999</v>
-      </c>
-      <c r="K130" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B131" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C131" s="11">
-        <v>9.9999999911233005E-3</v>
-      </c>
-      <c r="E131" s="11">
-        <v>69954.720000000001</v>
-      </c>
-      <c r="G131" s="11">
-        <f t="shared" si="4"/>
-        <v>58772.57</v>
-      </c>
-      <c r="I131" s="11">
-        <f t="shared" si="5"/>
-        <v>11182.16</v>
-      </c>
-      <c r="K131" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B132" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C132" s="11">
-        <v>0</v>
-      </c>
-      <c r="E132" s="11">
-        <v>25509.599999999999</v>
-      </c>
-      <c r="G132" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I132" s="11">
-        <f t="shared" si="5"/>
-        <v>25509.599999999999</v>
-      </c>
-      <c r="K132" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B133" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C133" s="11">
-        <v>152871.81817072001</v>
-      </c>
-      <c r="E133" s="11">
-        <v>125746.72</v>
-      </c>
-      <c r="G133" s="11">
-        <f t="shared" si="4"/>
-        <v>260889.39817072</v>
-      </c>
-      <c r="I133" s="11">
-        <f t="shared" si="5"/>
-        <v>17729.14</v>
-      </c>
-      <c r="K133" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B134" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C134" s="11">
-        <v>819630.83316300786</v>
-      </c>
-      <c r="E134" s="11">
-        <v>2589.5469118602</v>
-      </c>
-      <c r="G134" s="11">
-        <f t="shared" si="4"/>
-        <v>822220.38007487019</v>
-      </c>
-      <c r="I134" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K134" s="14">
-        <f t="shared" si="6"/>
-        <v>-2.0954757928848267E-9</v>
-      </c>
-    </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B135" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C135" s="11">
-        <v>33899.110709289998</v>
-      </c>
-      <c r="E135" s="11">
-        <v>910371.62056707998</v>
-      </c>
-      <c r="G135" s="11">
-        <f t="shared" si="4"/>
-        <v>97500.331276368001</v>
-      </c>
-      <c r="I135" s="11">
-        <f t="shared" si="5"/>
-        <v>846770.4</v>
-      </c>
-      <c r="K135" s="14">
-        <f t="shared" si="6"/>
-        <v>1.9790604710578918E-9</v>
-      </c>
-    </row>
-    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B136" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C136" s="11">
-        <v>7654.17</v>
-      </c>
-      <c r="E136" s="11">
-        <v>140326.23000000001</v>
-      </c>
-      <c r="G136" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I136" s="11">
-        <f t="shared" si="5"/>
-        <v>147980.4</v>
-      </c>
-      <c r="K136" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B137" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C137" s="11">
-        <v>0</v>
-      </c>
-      <c r="E137" s="11">
-        <v>21987.9</v>
-      </c>
-      <c r="G137" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I137" s="11">
-        <f t="shared" si="5"/>
-        <v>21987.9</v>
-      </c>
-      <c r="K137" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B138" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C138" s="11">
-        <v>184834.16817187</v>
-      </c>
-      <c r="E138" s="11">
-        <v>419320.78706465999</v>
-      </c>
-      <c r="G138" s="11">
-        <f t="shared" si="4"/>
-        <v>1971.6652365325001</v>
-      </c>
-      <c r="I138" s="11">
-        <f t="shared" si="5"/>
-        <v>602183.29</v>
-      </c>
-      <c r="K138" s="14">
-        <f t="shared" si="6"/>
-        <v>-2.5611370801925659E-9</v>
-      </c>
-    </row>
-    <row r="139" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B139" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C139" s="11">
-        <v>4019.8563611567001</v>
-      </c>
-      <c r="E139" s="11">
-        <v>4019.8563611567001</v>
-      </c>
-      <c r="G139" s="11">
-        <f t="shared" si="4"/>
-        <v>8039.7127223134003</v>
-      </c>
-      <c r="I139" s="11">
-        <f t="shared" si="5"/>
-        <v>2.8421709430404002E-13</v>
-      </c>
-      <c r="K139" s="14">
-        <f t="shared" si="6"/>
-        <v>-2.8421709430404002E-13</v>
-      </c>
-    </row>
-    <row r="140" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B140" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C140" s="11">
-        <v>7639.58</v>
-      </c>
-      <c r="D140" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E140" s="11">
-        <v>71713.460000000006</v>
-      </c>
-      <c r="F140" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="G140" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H140" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I140" s="11">
-        <f t="shared" si="5"/>
-        <v>79353.040000000008</v>
-      </c>
-      <c r="J140" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="K140" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B141" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C141" s="11">
-        <v>2151.29</v>
-      </c>
-      <c r="E141" s="11">
-        <v>12159.42</v>
-      </c>
-      <c r="G141" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I141" s="11">
-        <f t="shared" si="5"/>
-        <v>14310.71</v>
-      </c>
-      <c r="K141" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B142" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C142" s="11">
-        <v>81174.95</v>
-      </c>
-      <c r="E142" s="11">
-        <v>341568.97000000003</v>
-      </c>
-      <c r="G142" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I142" s="11">
-        <f t="shared" si="5"/>
-        <v>422743.92000000004</v>
-      </c>
-      <c r="K142" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B143" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C143" s="11">
-        <v>171696.38610903799</v>
-      </c>
-      <c r="E143" s="11">
-        <v>43278.246086077997</v>
-      </c>
-      <c r="G143" s="11">
-        <f t="shared" si="4"/>
-        <v>143559.632195118</v>
-      </c>
-      <c r="I143" s="11">
-        <f t="shared" si="5"/>
-        <v>71415</v>
-      </c>
-      <c r="K143" s="14">
-        <f t="shared" si="6"/>
-        <v>-2.0081643015146255E-9</v>
-      </c>
-    </row>
-    <row r="144" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B144" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C144" s="11">
-        <v>6084.0486357421996</v>
-      </c>
-      <c r="E144" s="11">
-        <v>6084.0486357421996</v>
-      </c>
-      <c r="G144" s="11">
-        <f t="shared" si="4"/>
-        <v>12168.097271484399</v>
-      </c>
-      <c r="I144" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K144" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B145" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C145" s="11">
-        <v>153694.62560423999</v>
-      </c>
-      <c r="E145" s="11">
-        <v>153694.62560423999</v>
-      </c>
-      <c r="G145" s="11">
-        <f t="shared" si="4"/>
-        <v>307389.25120847998</v>
-      </c>
-      <c r="I145" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K145" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B146" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C146" s="11">
-        <v>5958478.3042385401</v>
-      </c>
-      <c r="E146" s="11">
-        <v>5806603.9036335004</v>
-      </c>
-      <c r="G146" s="11">
-        <f t="shared" si="4"/>
-        <v>9163598.4678720273</v>
-      </c>
-      <c r="I146" s="11">
-        <f t="shared" si="5"/>
-        <v>2601483.7399999998</v>
-      </c>
-      <c r="K146" s="14">
-        <f t="shared" si="6"/>
-        <v>1.3504177331924438E-8</v>
-      </c>
-    </row>
-    <row r="147" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B147" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C147" s="11">
-        <v>0</v>
-      </c>
-      <c r="E147" s="11">
-        <v>204990.24277469399</v>
-      </c>
-      <c r="G147" s="11">
-        <f t="shared" si="4"/>
-        <v>204990.24277469999</v>
-      </c>
-      <c r="I147" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K147" s="14">
-        <f t="shared" si="6"/>
-        <v>-5.9953890740871429E-9</v>
-      </c>
-    </row>
-    <row r="148" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B148" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C148" s="11">
-        <v>2811.25</v>
-      </c>
-      <c r="E148" s="11">
-        <v>18338</v>
-      </c>
-      <c r="G148" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I148" s="11">
-        <f t="shared" si="5"/>
-        <v>21149.25</v>
-      </c>
-      <c r="K148" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B149" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C149" s="11">
-        <v>6765.2299368800996</v>
-      </c>
-      <c r="E149" s="11">
-        <v>114.77006311993</v>
-      </c>
-      <c r="G149" s="11">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I149" s="11">
-        <f t="shared" si="5"/>
-        <v>6880</v>
-      </c>
-      <c r="K149" s="14">
-        <f t="shared" si="6"/>
-        <v>2.9103830456733704E-11</v>
-      </c>
-    </row>
-    <row r="150" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B150" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C150" s="11">
-        <v>284929.50689949642</v>
-      </c>
-      <c r="E150" s="11">
-        <v>283520.52911790001</v>
-      </c>
-      <c r="G150" s="11">
-        <f t="shared" si="4"/>
-        <v>383681.03601740091</v>
-      </c>
-      <c r="I150" s="11">
-        <f t="shared" si="5"/>
-        <v>184769</v>
-      </c>
-      <c r="K150" s="14">
-        <f t="shared" si="6"/>
-        <v>-4.4237822294235229E-9</v>
-      </c>
-    </row>
-    <row r="151" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B151" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C151" s="11">
-        <v>0</v>
-      </c>
-      <c r="E151" s="11">
-        <v>39169.811628099</v>
-      </c>
-      <c r="G151" s="11">
-        <f t="shared" si="4"/>
-        <v>39169.811628099</v>
-      </c>
-      <c r="I151" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K151" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B152" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C152" s="11">
-        <v>68.315984670820995</v>
-      </c>
-      <c r="E152" s="11">
-        <v>68.315984670820995</v>
-      </c>
-      <c r="G152" s="11">
-        <f t="shared" si="4"/>
-        <v>136.63196934164199</v>
-      </c>
-      <c r="I152" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K152" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B153" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C153" s="11">
-        <v>3804</v>
-      </c>
-      <c r="E153" s="11">
-        <v>3804</v>
-      </c>
-      <c r="G153" s="11">
-        <f t="shared" si="4"/>
-        <v>3804</v>
-      </c>
-      <c r="I153" s="11">
-        <f t="shared" si="5"/>
-        <v>3804</v>
-      </c>
-      <c r="K153" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B154" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C154" s="11">
-        <v>35.955781405694999</v>
-      </c>
-      <c r="E154" s="11">
-        <v>35.955781405694999</v>
-      </c>
-      <c r="G154" s="11">
-        <f t="shared" si="4"/>
-        <v>71.911562811389999</v>
-      </c>
-      <c r="I154" s="11">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K154" s="14">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B155" s="13"/>
-      <c r="C155" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D155" s="12"/>
-      <c r="E155" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F155" s="12"/>
-      <c r="G155" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H155" s="12"/>
-      <c r="I155" s="12" t="s">
-        <v>92</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -13017,7 +11773,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="6">
-        <v>11595.754399777999</v>
+        <v>11595.754399778099</v>
       </c>
       <c r="AK10" s="6">
         <v>0</v>
@@ -13029,7 +11785,7 @@
         <v>0</v>
       </c>
       <c r="AN10" s="6">
-        <v>56051.467633337998</v>
+        <v>56051.467633338303</v>
       </c>
       <c r="AO10" s="6">
         <v>0</v>
@@ -13044,7 +11800,7 @@
         <v>0</v>
       </c>
       <c r="AS10" s="6">
-        <v>29853.109243252002</v>
+        <v>29853.1092432519</v>
       </c>
       <c r="AT10" s="6">
         <v>0</v>
@@ -14092,7 +12848,7 @@
         <v>0</v>
       </c>
       <c r="AI21" s="6">
-        <v>581757.91256396996</v>
+        <v>581757.91256396403</v>
       </c>
       <c r="AJ21" s="6">
         <v>0</v>
@@ -14612,7 +13368,7 @@
         <v>0</v>
       </c>
       <c r="AS26" s="6">
-        <v>40736.604093223003</v>
+        <v>40736.604093223199</v>
       </c>
       <c r="AT26" s="6">
         <v>0</v>
@@ -15086,7 +13842,7 @@
         <v>0</v>
       </c>
       <c r="AJ34" s="6">
-        <v>89681.660773001</v>
+        <v>89681.660773001393</v>
       </c>
       <c r="AK34" s="6">
         <v>0</v>
@@ -15368,7 +14124,7 @@
         <v>0</v>
       </c>
       <c r="AJ40" s="6">
-        <v>131982.08206096001</v>
+        <v>131982.08206096201</v>
       </c>
       <c r="AK40" s="6">
         <v>144560.68</v>
@@ -15439,10 +14195,10 @@
         <v>0</v>
       </c>
       <c r="AR41" s="6">
-        <v>2744.9197265717999</v>
+        <v>2744.9197265717698</v>
       </c>
       <c r="AS41" s="6">
-        <v>868808.68315278995</v>
+        <v>868808.683152791</v>
       </c>
       <c r="AT41" s="6">
         <v>0</v>
@@ -15615,7 +14371,7 @@
         <v>0</v>
       </c>
       <c r="AN45" s="6">
-        <v>2089.9651507243998</v>
+        <v>2089.9651507244198</v>
       </c>
       <c r="AO45" s="6">
         <v>0</v>
@@ -15662,10 +14418,10 @@
         <v>0</v>
       </c>
       <c r="AN46" s="6">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AO46" s="6">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AP46" s="6">
         <v>0</v>
@@ -15847,7 +14603,7 @@
         <v>0</v>
       </c>
       <c r="AM50" s="6">
-        <v>104292.6415534</v>
+        <v>104292.64155340299</v>
       </c>
       <c r="AN50" s="6">
         <v>0</v>
@@ -15856,7 +14612,7 @@
         <v>0</v>
       </c>
       <c r="AP50" s="6">
-        <v>45009.375929520997</v>
+        <v>45009.375929521302</v>
       </c>
       <c r="AQ50" s="6">
         <v>0</v>
@@ -15909,10 +14665,10 @@
         <v>0</v>
       </c>
       <c r="AR51" s="6">
-        <v>6327.4105811718</v>
+        <v>6327.41058117185</v>
       </c>
       <c r="AS51" s="6">
-        <v>6327.4105811718</v>
+        <v>6327.41058117185</v>
       </c>
       <c r="AT51" s="6">
         <v>0</v>
@@ -15947,13 +14703,13 @@
         <v>0</v>
       </c>
       <c r="AO52" s="6">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AP52" s="6">
         <v>0</v>
       </c>
       <c r="AQ52" s="6">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AR52" s="6">
         <v>0</v>
@@ -15976,22 +14732,22 @@
         <v>0</v>
       </c>
       <c r="AI53" s="6">
-        <v>221053.00971429</v>
+        <v>221053.00971429399</v>
       </c>
       <c r="AJ53" s="6">
-        <v>6157199.3426174996</v>
+        <v>6157199.3426175099</v>
       </c>
       <c r="AK53" s="6">
         <v>0</v>
       </c>
       <c r="AL53" s="6">
-        <v>86648.523400000005</v>
+        <v>86648.523399999802</v>
       </c>
       <c r="AM53" s="6">
         <v>0</v>
       </c>
       <c r="AN53" s="6">
-        <v>2666755.5876485002</v>
+        <v>2666755.58764851</v>
       </c>
       <c r="AO53" s="6">
         <v>0</v>
@@ -16056,7 +14812,7 @@
         <v>0</v>
       </c>
       <c r="AT54" s="6">
-        <v>217289.65734117999</v>
+        <v>217289.65734117699</v>
       </c>
     </row>
     <row r="55" spans="32:46" x14ac:dyDescent="0.2">
@@ -16179,7 +14935,7 @@
         <v>0</v>
       </c>
       <c r="AN57" s="6">
-        <v>4201.5329344260999</v>
+        <v>4201.5329344260599</v>
       </c>
       <c r="AO57" s="6">
         <v>326048.60848559003</v>
@@ -16276,7 +15032,7 @@
         <v>68.315984670820995</v>
       </c>
       <c r="AO59" s="6">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AP59" s="6">
         <v>0</v>
@@ -16367,10 +15123,10 @@
         <v>0</v>
       </c>
       <c r="AN61" s="6">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AO61" s="6">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AP61" s="6">
         <v>0</v>
@@ -16558,7 +15314,7 @@
         <v>0</v>
       </c>
       <c r="AJ66" s="5">
-        <v>89681.660773001</v>
+        <v>89681.660773001393</v>
       </c>
       <c r="AK66" s="5">
         <v>0</v>
@@ -16666,7 +15422,7 @@
         <v>0</v>
       </c>
       <c r="BV66" s="1">
-        <v>7295.5878000000002</v>
+        <v>7295.5878000000203</v>
       </c>
       <c r="BW66" s="1">
         <v>0</v>
@@ -16803,7 +15559,7 @@
         <v>0</v>
       </c>
       <c r="BV67" s="1">
-        <v>1.0600000000111E-2</v>
+        <v>1.0600000000110899E-2</v>
       </c>
       <c r="BW67" s="1">
         <v>0</v>
@@ -17380,7 +16136,7 @@
         <v>0</v>
       </c>
       <c r="AJ72" s="5">
-        <v>131982.08206096001</v>
+        <v>131982.08206096201</v>
       </c>
       <c r="AK72" s="5">
         <v>144560.68</v>
@@ -17541,10 +16297,10 @@
         <v>0</v>
       </c>
       <c r="AR73" s="5">
-        <v>2744.9197265717999</v>
+        <v>2744.9197265717698</v>
       </c>
       <c r="AS73" s="5">
-        <v>868808.68315278995</v>
+        <v>868808.683152791</v>
       </c>
       <c r="AT73" s="5">
         <v>0</v>
@@ -17654,7 +16410,7 @@
         <v>0</v>
       </c>
       <c r="AJ74" s="5">
-        <v>11595.754399777999</v>
+        <v>11595.754399778099</v>
       </c>
       <c r="AK74" s="5">
         <v>0</v>
@@ -17666,7 +16422,7 @@
         <v>0</v>
       </c>
       <c r="AN74" s="5">
-        <v>56051.467633337998</v>
+        <v>56051.467633338303</v>
       </c>
       <c r="AO74" s="5">
         <v>0</v>
@@ -17681,7 +16437,7 @@
         <v>0</v>
       </c>
       <c r="AS74" s="5">
-        <v>29853.109243252002</v>
+        <v>29853.1092432519</v>
       </c>
       <c r="AT74" s="5">
         <v>0</v>
@@ -17762,7 +16518,7 @@
         <v>104.4</v>
       </c>
       <c r="BV74" s="1">
-        <v>10774.8</v>
+        <v>10774.799999999899</v>
       </c>
       <c r="BW74" s="1">
         <v>450</v>
@@ -18036,7 +16792,7 @@
         <v>0</v>
       </c>
       <c r="BV76" s="1">
-        <v>3.7834979593754002E-12</v>
+        <v>3.78349795937538E-12</v>
       </c>
       <c r="BW76" s="1">
         <v>0</v>
@@ -18077,7 +16833,7 @@
         <v>0</v>
       </c>
       <c r="AN77" s="5">
-        <v>2089.9651507243998</v>
+        <v>2089.9651507244198</v>
       </c>
       <c r="AO77" s="5">
         <v>0</v>
@@ -18173,7 +16929,7 @@
         <v>362463.5232</v>
       </c>
       <c r="BV77" s="1">
-        <v>2.1199999958043999E-2</v>
+        <v>2.1199999958043898E-2</v>
       </c>
       <c r="BW77" s="1">
         <v>0</v>
@@ -18214,10 +16970,10 @@
         <v>0</v>
       </c>
       <c r="AN78" s="5">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AO78" s="5">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="AP78" s="5">
         <v>0</v>
@@ -18447,7 +17203,7 @@
         <v>0</v>
       </c>
       <c r="BV79" s="1">
-        <v>7.7125150710343995E-12</v>
+        <v>7.7125150710344302E-12</v>
       </c>
       <c r="BW79" s="1">
         <v>0</v>
@@ -18759,7 +17515,7 @@
         <v>0</v>
       </c>
       <c r="AM82" s="5">
-        <v>104292.6415534</v>
+        <v>104292.64155340299</v>
       </c>
       <c r="AN82" s="5">
         <v>0</v>
@@ -18768,7 +17524,7 @@
         <v>0</v>
       </c>
       <c r="AP82" s="5">
-        <v>45009.375929520997</v>
+        <v>45009.375929521302</v>
       </c>
       <c r="AQ82" s="5">
         <v>0</v>
@@ -18858,7 +17614,7 @@
         <v>7.4880000000000004</v>
       </c>
       <c r="BV82" s="1">
-        <v>1.5133991837502001E-11</v>
+        <v>1.5133991837501501E-11</v>
       </c>
       <c r="BW82" s="1">
         <v>9.36</v>
@@ -18911,10 +17667,10 @@
         <v>0</v>
       </c>
       <c r="AR83" s="5">
-        <v>6327.4105811718</v>
+        <v>6327.41058117185</v>
       </c>
       <c r="AS83" s="5">
-        <v>6327.4105811718</v>
+        <v>6327.41058117185</v>
       </c>
       <c r="AT83" s="5">
         <v>0</v>
@@ -19039,13 +17795,13 @@
         <v>0</v>
       </c>
       <c r="AO84" s="5">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AP84" s="5">
         <v>0</v>
       </c>
       <c r="AQ84" s="5">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="AR84" s="5">
         <v>0</v>
@@ -19158,22 +17914,22 @@
         <v>0</v>
       </c>
       <c r="AI85" s="5">
-        <v>802810.92227826</v>
+        <v>802810.92227825697</v>
       </c>
       <c r="AJ85" s="5">
-        <v>6157199.3426174996</v>
+        <v>6157199.3426175099</v>
       </c>
       <c r="AK85" s="5">
         <v>0</v>
       </c>
       <c r="AL85" s="5">
-        <v>86648.523400000005</v>
+        <v>86648.523399999802</v>
       </c>
       <c r="AM85" s="5">
         <v>0</v>
       </c>
       <c r="AN85" s="5">
-        <v>2666755.5876485002</v>
+        <v>2666755.58764851</v>
       </c>
       <c r="AO85" s="5">
         <v>0</v>
@@ -19328,7 +18084,7 @@
         <v>0</v>
       </c>
       <c r="AT86" s="5">
-        <v>217289.65734117999</v>
+        <v>217289.65734117699</v>
       </c>
       <c r="AW86" s="4" t="s">
         <v>21</v>
@@ -19721,7 +18477,7 @@
         <v>0</v>
       </c>
       <c r="AN89" s="5">
-        <v>4201.5329344260999</v>
+        <v>4201.5329344260599</v>
       </c>
       <c r="AO89" s="5">
         <v>326048.60848559003</v>
@@ -19873,7 +18629,7 @@
         <v>0</v>
       </c>
       <c r="AS90" s="5">
-        <v>40736.604093223003</v>
+        <v>40736.604093223199</v>
       </c>
       <c r="AT90" s="5">
         <v>0</v>
@@ -19998,7 +18754,7 @@
         <v>68.315984670820995</v>
       </c>
       <c r="AO91" s="5">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AP91" s="5">
         <v>0</v>
@@ -20269,10 +19025,10 @@
         <v>0</v>
       </c>
       <c r="AN93" s="5">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AO93" s="5">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
       <c r="AP93" s="5">
         <v>0</v>
@@ -20763,7 +19519,7 @@
         <v>0</v>
       </c>
       <c r="V100" s="5">
-        <v>160637.14537576999</v>
+        <v>160637.145375767</v>
       </c>
       <c r="W100" s="5">
         <v>0</v>
@@ -20849,7 +19605,7 @@
         <v>0</v>
       </c>
       <c r="U101" s="5">
-        <v>6155000.1378515</v>
+        <v>6155000.1378514804</v>
       </c>
       <c r="V101" s="5">
         <v>0</v>
@@ -21119,7 +19875,7 @@
         <v>0</v>
       </c>
       <c r="V104" s="5">
-        <v>56652.511965411002</v>
+        <v>56652.511965410798</v>
       </c>
       <c r="W104" s="5">
         <v>0</v>
@@ -21172,7 +19928,7 @@
         <v>0</v>
       </c>
       <c r="J105" s="5">
-        <v>859652.39411768003</v>
+        <v>859652.39411767898</v>
       </c>
       <c r="K105" s="5">
         <v>0</v>
@@ -21273,7 +20029,7 @@
         <v>0</v>
       </c>
       <c r="N106" s="5">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="O106" s="5">
         <v>0</v>
@@ -21291,7 +20047,7 @@
         <v>0</v>
       </c>
       <c r="T106" s="5">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="U106" s="5">
         <v>0</v>
@@ -21312,13 +20068,13 @@
         <v>0</v>
       </c>
       <c r="AA106" s="5">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AB106" s="5">
         <v>951</v>
       </c>
       <c r="AC106" s="5">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.2">
@@ -21374,7 +20130,7 @@
         <v>0</v>
       </c>
       <c r="R107" s="5">
-        <v>45009.375929520997</v>
+        <v>45009.375929521302</v>
       </c>
       <c r="S107" s="5">
         <v>0</v>
@@ -21439,7 +20195,7 @@
         <v>0</v>
       </c>
       <c r="J108" s="5">
-        <v>50719.226449399997</v>
+        <v>50719.226449399699</v>
       </c>
       <c r="K108" s="5">
         <v>0</v>
@@ -21525,7 +20281,7 @@
         <v>0</v>
       </c>
       <c r="I109" s="5">
-        <v>2744.9197265717999</v>
+        <v>2744.9197265717698</v>
       </c>
       <c r="J109" s="5">
         <v>0</v>
@@ -21555,7 +20311,7 @@
         <v>0</v>
       </c>
       <c r="S109" s="5">
-        <v>6327.4105811718</v>
+        <v>6327.41058117184</v>
       </c>
       <c r="T109" s="5">
         <v>0</v>
@@ -21626,7 +20382,7 @@
         <v>0</v>
       </c>
       <c r="M110" s="5">
-        <v>320884.46673679998</v>
+        <v>320884.46673680301</v>
       </c>
       <c r="N110" s="5">
         <v>0</v>
@@ -21659,13 +20415,13 @@
         <v>19438.28</v>
       </c>
       <c r="X110" s="5">
-        <v>121.65626690712</v>
+        <v>121.65626690712401</v>
       </c>
       <c r="Y110" s="5">
         <v>0</v>
       </c>
       <c r="Z110" s="5">
-        <v>40736.604093223003</v>
+        <v>40736.604093223199</v>
       </c>
       <c r="AA110" s="5">
         <v>0</v>
@@ -21715,7 +20471,7 @@
         <v>0</v>
       </c>
       <c r="M111" s="5">
-        <v>123595.56755173999</v>
+        <v>123595.56755173601</v>
       </c>
       <c r="N111" s="5">
         <v>0</v>
@@ -21914,34 +20670,34 @@
         <v>30062.0452</v>
       </c>
       <c r="I116" s="1">
-        <v>775980.48876326997</v>
+        <v>775980.488763273</v>
       </c>
       <c r="J116" s="1">
-        <v>33899.110709289002</v>
+        <v>33899.110709289402</v>
       </c>
       <c r="K116" s="1">
-        <v>4699.5735999999997</v>
+        <v>4699.5735999999897</v>
       </c>
       <c r="L116" s="1">
         <v>0</v>
       </c>
       <c r="M116" s="1">
-        <v>195924.21826219</v>
+        <v>195924.21826218601</v>
       </c>
       <c r="N116" s="1">
         <v>0</v>
       </c>
       <c r="O116" s="1">
-        <v>8097.9548000000004</v>
+        <v>8097.9548000000104</v>
       </c>
       <c r="P116" s="1">
         <v>1982.9208000000001</v>
       </c>
       <c r="Q116" s="1">
-        <v>52103.4732</v>
+        <v>52103.473200000102</v>
       </c>
       <c r="R116" s="1">
-        <v>133554.86562388</v>
+        <v>133554.86562388201</v>
       </c>
       <c r="S116" s="1">
         <v>0</v>
@@ -21959,10 +20715,10 @@
         <v>0</v>
       </c>
       <c r="X116" s="1">
-        <v>7171.1437330929002</v>
+        <v>7171.1437330928802</v>
       </c>
       <c r="Y116" s="1">
-        <v>1620.3244488358</v>
+        <v>1620.3244488358901</v>
       </c>
       <c r="Z116" s="1">
         <v>0</v>
@@ -21982,7 +20738,7 @@
         <v>30</v>
       </c>
       <c r="B117" s="1">
-        <v>89681.660773001</v>
+        <v>89681.660773001393</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -22000,10 +20756,10 @@
         <v>0</v>
       </c>
       <c r="H117" s="1">
-        <v>131982.08206096001</v>
+        <v>131982.08206096201</v>
       </c>
       <c r="I117" s="1">
-        <v>2744.9197265717999</v>
+        <v>2744.9197265717698</v>
       </c>
       <c r="J117" s="1">
         <v>0</v>
@@ -22018,7 +20774,7 @@
         <v>0</v>
       </c>
       <c r="N117" s="1">
-        <v>4019.8563611567001</v>
+        <v>4019.8563611567301</v>
       </c>
       <c r="O117" s="1">
         <v>0</v>
@@ -22030,16 +20786,16 @@
         <v>0</v>
       </c>
       <c r="R117" s="1">
-        <v>45009.375929520997</v>
+        <v>45009.375929521302</v>
       </c>
       <c r="S117" s="1">
-        <v>6327.4105811718</v>
+        <v>6327.41058117185</v>
       </c>
       <c r="T117" s="1">
-        <v>153694.62560423999</v>
+        <v>153694.625604242</v>
       </c>
       <c r="U117" s="1">
-        <v>6157199.3426174996</v>
+        <v>6157199.3426175099</v>
       </c>
       <c r="V117" s="1">
         <v>0</v>
@@ -22057,13 +20813,13 @@
         <v>0</v>
       </c>
       <c r="AA117" s="1">
-        <v>68.315984670820995</v>
+        <v>68.315984670820896</v>
       </c>
       <c r="AB117" s="1">
         <v>951</v>
       </c>
       <c r="AC117" s="1">
-        <v>35.955781405694999</v>
+        <v>35.955781405695198</v>
       </c>
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.2">
@@ -22083,7 +20839,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="1">
-        <v>1.050000000032E-2</v>
+        <v>1.0500000014872101E-2</v>
       </c>
       <c r="G118" s="1">
         <v>0</v>
@@ -22092,13 +20848,13 @@
         <v>0</v>
       </c>
       <c r="I118" s="1">
-        <v>84094.358895879996</v>
+        <v>84094.358895880505</v>
       </c>
       <c r="J118" s="1">
         <v>0</v>
       </c>
       <c r="K118" s="1">
-        <v>3413.8465999999999</v>
+        <v>3413.8465999999798</v>
       </c>
       <c r="L118" s="1">
         <v>0</v>
@@ -22128,10 +20884,10 @@
         <v>0</v>
       </c>
       <c r="U118" s="1">
-        <v>158787.65987529</v>
+        <v>158787.659875296</v>
       </c>
       <c r="V118" s="1">
-        <v>0</v>
+        <v>-2.91038304567337E-11</v>
       </c>
       <c r="W118" s="1">
         <v>2979.9250000000002</v>
@@ -22181,7 +20937,7 @@
         <v>0</v>
       </c>
       <c r="I119" s="1">
-        <v>5988.9157670656996</v>
+        <v>5988.9157670656696</v>
       </c>
       <c r="J119" s="1">
         <v>0</v>

</xml_diff>